<commit_message>
added comments and hours
</commit_message>
<xml_diff>
--- a/documentation/project2_hours_team9.xlsx
+++ b/documentation/project2_hours_team9.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric Z\Desktop\Battleship Game Project 1 EECS448\eecs448-project-2\battleship\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duy Vu\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4B331D-54FE-46FD-B681-35B8DC17335E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085A354C-9176-4D55-8C5C-1E0E9A89D720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3195" yWindow="2565" windowWidth="21600" windowHeight="11385" xr2:uid="{DE4D3226-987C-D248-9F68-E3A41E1223A4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DE4D3226-987C-D248-9F68-E3A41E1223A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
   <si>
     <t>Hour Tracking - Project 2</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Eric</t>
+  </si>
+  <si>
+    <t>Duy</t>
   </si>
 </sst>
 </file>
@@ -422,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB7A24C7-8340-4F46-BF5B-ECA2B5254AA8}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -483,13 +486,13 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1">
-        <v>44620</v>
+        <v>44617</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -497,10 +500,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="1">
-        <v>44621</v>
+        <v>44620</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -508,74 +511,118 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>44622</v>
+        <v>44621</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1">
         <v>44622</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>44623</v>
+        <v>44622</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1">
-        <v>44623</v>
+        <v>44622</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="1">
-        <v>44624</v>
+        <v>44623</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1">
+        <v>44623</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1">
+        <v>44623</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44624</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="1">
+        <v>44624</v>
+      </c>
+      <c r="C16">
         <v>4</v>
       </c>
-      <c r="B13" s="1">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1">
         <v>44624</v>
       </c>
-      <c r="C13">
+      <c r="C17">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C33">
-        <f>SUM(C3:C32)</f>
-        <v>32.5</v>
+      <c r="C37">
+        <f>SUM(C3:C36)</f>
+        <v>44.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>